<commit_message>
The Curious: Correlation Coefficient
</commit_message>
<xml_diff>
--- a/The Curious/worksheet.xlsx
+++ b/The Curious/worksheet.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eskim\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codes\data-analyst\The Curious\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFFE514-A387-45B2-BB45-C8861DC88985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB3C6D0-A218-4F59-B781-82E6850A9AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{32FAD7BD-02B4-48F7-822D-E535DEF6A923}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{32FAD7BD-02B4-48F7-822D-E535DEF6A923}"/>
   </bookViews>
   <sheets>
     <sheet name="Correlation" sheetId="1" r:id="rId1"/>
@@ -32,8 +32,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
   <si>
     <t>Sales</t>
   </si>
@@ -221,13 +219,22 @@
   </si>
   <si>
     <t>SLOPE</t>
+  </si>
+  <si>
+    <t>SD_Ad</t>
+  </si>
+  <si>
+    <t>SD_Sale</t>
+  </si>
+  <si>
+    <t>Manual COR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,6 +305,949 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Correlation!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Correlation!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Correlation!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7FD6-4E94-870C-82932FCD3160}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="193299519"/>
+        <c:axId val="238711407"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="193299519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="238711407"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="238711407"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="193299519"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>45552</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>44727</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>327161</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>120927</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE298018-6591-509A-FA5B-4A60C7257505}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -617,18 +1567,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64177D66-829F-4BF3-B32C-B0FFD91CD2D5}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -636,7 +1586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.5</v>
       </c>
@@ -646,9 +1596,16 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2" s="1">
+        <f>_xlfn.COVARIANCE.S(A2:A9, B2:B9)</f>
+        <v>198.42857142857142</v>
+      </c>
+      <c r="F2" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E2)</f>
+        <v>=COVARIANCE.S(A2:A9, B2:B9)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -658,9 +1615,16 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3" s="1">
+        <f>CORREL(A2:A9, B2:B9)</f>
+        <v>0.96510847734580996</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F7" ca="1" si="0">_xlfn.FORMULATEXT(E3)</f>
+        <v>=CORREL(A2:A9, B2:B9)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2.2000000000000002</v>
       </c>
@@ -670,9 +1634,16 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4" s="1">
+        <f>E3^2</f>
+        <v>0.93143437304474774</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=E3^2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2.5</v>
       </c>
@@ -680,44 +1651,86 @@
         <v>720</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6">
         <v>850</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6">
+        <f>_xlfn.STDEV.S(A2:A9)</f>
+        <v>1.2282391577259826</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=STDEV.S(A2:A9)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7">
         <v>900</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="D7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7">
+        <f>_xlfn.STDEV.S(B2:B9)</f>
+        <v>167.39602316491445</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=STDEV.S(B2:B9)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4.2</v>
       </c>
       <c r="B8">
         <v>920</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="E8">
+        <f>E6*E7</f>
+        <v>205.60235049875359</v>
+      </c>
+      <c r="F8" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E8)</f>
+        <v>=E6*E7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9">
         <v>1000</v>
       </c>
-    </row>
-    <row r="25" spans="2:2">
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9">
+        <f>E2/E8</f>
+        <v>0.96510847734580896</v>
+      </c>
+      <c r="F9" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E9)</f>
+        <v>=E2/E8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -725,13 +1738,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04297F7D-16FE-4B61-89B2-B332F39E7985}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -757,7 +1770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.5</v>
       </c>
@@ -780,7 +1793,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -803,7 +1816,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2.2000000000000002</v>
       </c>
@@ -826,7 +1839,7 @@
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2.5</v>
       </c>
@@ -849,7 +1862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -863,7 +1876,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -877,7 +1890,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4.2</v>
       </c>
@@ -891,7 +1904,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -918,12 +1931,12 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -931,7 +1944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.5</v>
       </c>
@@ -943,7 +1956,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -955,7 +1968,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2.2000000000000002</v>
       </c>
@@ -967,7 +1980,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2.5</v>
       </c>
@@ -975,7 +1988,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -987,7 +2000,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -999,7 +2012,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4.2</v>
       </c>
@@ -1007,7 +2020,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1019,7 +2032,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="25" spans="2:2">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
     </row>
   </sheetData>
@@ -1036,9 +2049,9 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1052,7 +2065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.5</v>
       </c>
@@ -1066,7 +2079,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1080,7 +2093,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2.2000000000000002</v>
       </c>
@@ -1094,7 +2107,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2.5</v>
       </c>
@@ -1108,7 +2121,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1122,7 +2135,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1136,7 +2149,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4.2</v>
       </c>
@@ -1150,7 +2163,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1177,9 +2190,9 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1217,7 +2230,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1255,7 +2268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1293,7 +2306,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1331,7 +2344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1369,7 +2382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1407,7 +2420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1445,7 +2458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1483,7 +2496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1521,7 +2534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1559,7 +2572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1597,7 +2610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1635,7 +2648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1673,7 +2686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1711,7 +2724,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1749,7 +2762,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1787,7 +2800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1825,7 +2838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1863,7 +2876,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1901,7 +2914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1939,7 +2952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1977,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -2015,7 +3028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -2053,7 +3066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -2091,7 +3104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -2129,7 +3142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -2167,7 +3180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -2205,7 +3218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -2243,7 +3256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -2281,7 +3294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -2319,7 +3332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -2357,7 +3370,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -2395,7 +3408,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -2446,19 +3459,19 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -2469,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5">
         <v>2</v>
@@ -2478,7 +3491,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6">
         <v>2.2000000000000002</v>
@@ -2487,7 +3500,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7">
         <v>2.5</v>
@@ -2496,7 +3509,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8">
         <v>3</v>
@@ -2505,7 +3518,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9">
         <v>4</v>
@@ -2514,7 +3527,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10">
         <v>4.2</v>
@@ -2523,7 +3536,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11">
         <v>4.5999999999999996</v>
@@ -2532,7 +3545,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12">
         <v>5</v>
@@ -2541,7 +3554,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13">
         <v>5.0999999999999996</v>
@@ -2550,7 +3563,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14">
         <v>5.2</v>
@@ -2559,12 +3572,12 @@
         <v>190</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -2572,7 +3585,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2580,7 +3593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2.2000000000000002</v>
       </c>
@@ -2588,7 +3601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2596,7 +3609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3.5</v>
       </c>
@@ -2604,7 +3617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1.8</v>
       </c>
@@ -2612,7 +3625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>5</v>
       </c>
@@ -2620,7 +3633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5.6</v>
       </c>
@@ -2628,7 +3641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
@@ -2636,7 +3649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5.2</v>
       </c>
@@ -2644,7 +3657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5.4</v>
       </c>

</xml_diff>

<commit_message>
The Curious: Correlation Matrix
</commit_message>
<xml_diff>
--- a/The Curious/worksheet.xlsx
+++ b/The Curious/worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codes\data-analyst\The Curious\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB3C6D0-A218-4F59-B781-82E6850A9AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F35DCF9-FDD5-4D1C-8940-9B7D8625E83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{32FAD7BD-02B4-48F7-822D-E535DEF6A923}"/>
   </bookViews>
@@ -1739,7 +1739,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1809,7 +1809,10 @@
       <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1">
+        <f>CORREL(A2:A9, B2:B9)</f>
+        <v>0.97898592299729303</v>
+      </c>
       <c r="H3">
         <v>1</v>
       </c>
@@ -1832,8 +1835,14 @@
       <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="G4" s="1">
+        <f>CORREL(A2:A9, C2:C9)</f>
+        <v>0.94715654795825122</v>
+      </c>
+      <c r="H4" s="1">
+        <f>CORREL(B2:B9, C2:C9)</f>
+        <v>0.96139161026652109</v>
+      </c>
       <c r="I4">
         <v>1</v>
       </c>
@@ -1855,9 +1864,18 @@
       <c r="F5" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="G5" s="1">
+        <f>CORREL(A2:A9, D2:D9)</f>
+        <v>0.96510847734580996</v>
+      </c>
+      <c r="H5" s="1">
+        <f>CORREL(B2:B9, D2:D9)</f>
+        <v>0.96479411410647209</v>
+      </c>
+      <c r="I5" s="1">
+        <f>CORREL(C2:C9, D2:D9)</f>
+        <v>0.96149570908049409</v>
+      </c>
       <c r="J5">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
The Curious: Correlation Matrix upper cross
</commit_message>
<xml_diff>
--- a/The Curious/worksheet.xlsx
+++ b/The Curious/worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codes\data-analyst\The Curious\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F35DCF9-FDD5-4D1C-8940-9B7D8625E83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22D3A29-4DB1-4934-87F3-D9EEFA203E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{32FAD7BD-02B4-48F7-822D-E535DEF6A923}"/>
   </bookViews>
@@ -1739,7 +1739,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1789,9 +1789,18 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="H2" s="2">
+        <f>CORREL(B2:B9, A2:A9)</f>
+        <v>0.97898592299729303</v>
+      </c>
+      <c r="I2" s="2">
+        <f>CORREL(C2:C9, A2:A9)</f>
+        <v>0.94715654795825122</v>
+      </c>
+      <c r="J2" s="2">
+        <f>CORREL(D2:D9, A2:A9)</f>
+        <v>0.96510847734580996</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1816,8 +1825,14 @@
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="I3" s="2">
+        <f>CORREL(C2:C9, B2:B9)</f>
+        <v>0.96139161026652109</v>
+      </c>
+      <c r="J3" s="2">
+        <f>CORREL(D2:D9, B2:B9)</f>
+        <v>0.96479411410647209</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1846,7 +1861,10 @@
       <c r="I4">
         <v>1</v>
       </c>
-      <c r="J4" s="2"/>
+      <c r="J4" s="2">
+        <f>CORREL(D2:D9, C2:C9)</f>
+        <v>0.96149570908049409</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">

</xml_diff>

<commit_message>
The Curious: Simple Linear Regression (SLR)
</commit_message>
<xml_diff>
--- a/The Curious/worksheet.xlsx
+++ b/The Curious/worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codes\data-analyst\The Curious\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22D3A29-4DB1-4934-87F3-D9EEFA203E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D81DDC-E823-4145-90EE-AD3400F736C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{32FAD7BD-02B4-48F7-822D-E535DEF6A923}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="2" xr2:uid="{32FAD7BD-02B4-48F7-822D-E535DEF6A923}"/>
   </bookViews>
   <sheets>
     <sheet name="Correlation" sheetId="1" r:id="rId1"/>
@@ -38,8 +38,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="67">
   <si>
     <t>Sales</t>
   </si>
@@ -228,12 +250,27 @@
   </si>
   <si>
     <t>Manual COR</t>
+  </si>
+  <si>
+    <t>SSm</t>
+  </si>
+  <si>
+    <t>SSr</t>
+  </si>
+  <si>
+    <t>SSt</t>
+  </si>
+  <si>
+    <t>R-Suared</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,7 +288,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,6 +307,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -284,11 +327,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -653,7 +699,437 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SLR!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SLR!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SLR!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7BA1-4388-8348-32E60833C219}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="885556063"/>
+        <c:axId val="885264415"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="885556063"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="885264415"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="885264415"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="885556063"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1209,6 +1685,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1230,6 +2222,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE298018-6591-509A-FA5B-4A60C7257505}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1288A9A9-3235-491B-34BC-3635708BFB90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1738,7 +2771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04297F7D-16FE-4B61-89B2-B332F39E7985}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -1961,18 +2994,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBCC879-4338-44AA-99E2-5CC879539C01}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1980,7 +3015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.5</v>
       </c>
@@ -1990,9 +3025,17 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="4">
+        <f>_xlfn.COVARIANCE.S(A2:A9, B2:B9)</f>
+        <v>198.42857142857142</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E2)</f>
+        <v>=COVARIANCE.S(A2:A9, B2:B9)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2002,9 +3045,17 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="4">
+        <f>CORREL(A2:A9, B2:B9)</f>
+        <v>0.96510847734580996</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E3)</f>
+        <v>=CORREL(A2:A9, B2:B9)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2.2000000000000002</v>
       </c>
@@ -2014,17 +3065,27 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="4">
+        <f>E3^2</f>
+        <v>0.93143437304474774</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E4)</f>
+        <v>=E3^2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2.5</v>
       </c>
       <c r="B5">
         <v>720</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2034,9 +3095,17 @@
       <c r="D6" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="4">
+        <f>INTERCEPT(B2:B9, A2:A9)</f>
+        <v>376.32102272727275</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E6)</f>
+        <v>=INTERCEPT(B2:B9, A2:A9)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2046,17 +3115,31 @@
       <c r="D7" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="4">
+        <f>SLOPE(B2:B9, A2:A9)</f>
+        <v>131.53409090909091</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E7)</f>
+        <v>=SLOPE(B2:B9, A2:A9)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4.2</v>
       </c>
       <c r="B8">
         <v>920</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2066,7 +3149,90 @@
       <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="4" cm="1">
+        <f t="array" ref="E9:F13">LINEST(B2:B9, A2:A9, TRUE, TRUE)</f>
+        <v>131.53409090909091</v>
+      </c>
+      <c r="F9" s="5">
+        <v>376.32102272727275</v>
+      </c>
+      <c r="G9" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E9)</f>
+        <v>=LINEST(B2:B9, A2:A9, TRUE, TRUE)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>14.569337292064308</v>
+      </c>
+      <c r="F10">
+        <v>47.484641943819497</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.93143437304474774</v>
+      </c>
+      <c r="F11">
+        <v>47.34474227633013</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>81.507403730381682</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>182700.85227272726</v>
+      </c>
+      <c r="F13">
+        <v>13449.147727272728</v>
+      </c>
+      <c r="G13">
+        <f>E13+F13</f>
+        <v>196150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="6">
+        <f>E13/G13</f>
+        <v>0.93143437304474774</v>
+      </c>
+      <c r="F15" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E15)</f>
+        <v>=E13/G13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="6">
+        <f>1-F13/G13</f>
+        <v>0.93143437304474774</v>
+      </c>
+      <c r="F16" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E16)</f>
+        <v>=1-F13/G13</v>
+      </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
@@ -2074,6 +3240,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
The Curious: Multiple Linear Regression (MLR)
</commit_message>
<xml_diff>
--- a/The Curious/worksheet.xlsx
+++ b/The Curious/worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codes\data-analyst\The Curious\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D81DDC-E823-4145-90EE-AD3400F736C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393556C4-3C2C-4D62-BFB2-03665ED04D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="2" xr2:uid="{32FAD7BD-02B4-48F7-822D-E535DEF6A923}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="3" xr2:uid="{32FAD7BD-02B4-48F7-822D-E535DEF6A923}"/>
   </bookViews>
   <sheets>
     <sheet name="Correlation" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
   <si>
     <t>Sales</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>R-Suared</t>
+  </si>
+  <si>
+    <t>Intercept</t>
   </si>
 </sst>
 </file>
@@ -269,7 +272,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -332,8 +335,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -2996,7 +2999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBCC879-4338-44AA-99E2-5CC879539C01}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -3246,15 +3249,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDF8118-C29E-43AF-A49E-80CFF0A01254}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3267,8 +3270,20 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.5</v>
       </c>
@@ -3281,8 +3296,21 @@
       <c r="D2">
         <v>500</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" cm="1">
+        <f t="array" ref="F2:I6">LINEST(D2:D9, A2:C9, TRUE, TRUE)</f>
+        <v>62.601508347545824</v>
+      </c>
+      <c r="G2">
+        <v>33.695686188606089</v>
+      </c>
+      <c r="H2">
+        <v>59.377102533210191</v>
+      </c>
+      <c r="I2">
+        <v>403.91477992833802</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3295,8 +3323,20 @@
       <c r="D3">
         <v>650</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>59.356685502743602</v>
+      </c>
+      <c r="G3">
+        <v>148.33428763107136</v>
+      </c>
+      <c r="H3">
+        <v>72.193180863079974</v>
+      </c>
+      <c r="I3">
+        <v>91.855799919147188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2.2000000000000002</v>
       </c>
@@ -3309,8 +3349,20 @@
       <c r="D4">
         <v>680</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" s="6">
+        <v>0.95385319143604363</v>
+      </c>
+      <c r="G4">
+        <v>47.570202069730733</v>
+      </c>
+      <c r="H4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2.5</v>
       </c>
@@ -3323,8 +3375,20 @@
       <c r="D5">
         <v>720</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>27.559961237306823</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -3337,8 +3401,20 @@
       <c r="D6">
         <v>850</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>187098.30350017996</v>
+      </c>
+      <c r="G6">
+        <v>9051.6964998200565</v>
+      </c>
+      <c r="H6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -3351,8 +3427,17 @@
       <c r="D7">
         <v>900</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4.2</v>
       </c>
@@ -3365,8 +3450,12 @@
       <c r="D8">
         <v>920</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f>F6+G6</f>
+        <v>196150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -3378,6 +3467,14 @@
       </c>
       <c r="D9">
         <v>1000</v>
+      </c>
+      <c r="F9" s="6">
+        <f>F6/H8</f>
+        <v>0.95385319143604363</v>
+      </c>
+      <c r="G9" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(F9)</f>
+        <v>=F6/H8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The Curious: Full Regression Result in Excel using Analysis Toolpak
</commit_message>
<xml_diff>
--- a/The Curious/worksheet.xlsx
+++ b/The Curious/worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codes\data-analyst\The Curious\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393556C4-3C2C-4D62-BFB2-03665ED04D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C67BF9-59FE-41FA-887D-A6A28A604887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="3" xr2:uid="{32FAD7BD-02B4-48F7-822D-E535DEF6A923}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="4" xr2:uid="{32FAD7BD-02B4-48F7-822D-E535DEF6A923}"/>
   </bookViews>
   <sheets>
     <sheet name="Correlation" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="93">
   <si>
     <t>Sales</t>
   </si>
@@ -265,6 +265,81 @@
   </si>
   <si>
     <t>Intercept</t>
+  </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
+  </si>
+  <si>
+    <t>การทดสอบ Overall Significance of the Model</t>
+  </si>
+  <si>
+    <t>&lt; 0.05</t>
   </si>
 </sst>
 </file>
@@ -274,7 +349,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,8 +365,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,8 +399,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -325,12 +420,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -338,6 +453,27 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3251,7 +3387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDF8118-C29E-43AF-A49E-80CFF0A01254}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -3484,15 +3620,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D7971B4-24C8-41D7-A24D-6C5A84F057BD}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="12" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -3530,7 +3672,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -3567,8 +3709,11 @@
       <c r="L2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -3606,7 +3751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -3643,8 +3788,12 @@
       <c r="L4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="O4" s="10"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -3681,8 +3830,14 @@
       <c r="L5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="O5" s="7">
+        <v>0.91645529354564448</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -3719,8 +3874,14 @@
       <c r="L6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N6" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="O6" s="11">
+        <v>0.83989030506783335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -3757,8 +3918,14 @@
       <c r="L7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N7" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O7" s="7">
+        <v>0.82273569489652976</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -3795,8 +3962,14 @@
       <c r="L8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="O8" s="7">
+        <v>2.5375119399426995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -3833,8 +4006,14 @@
       <c r="L9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N9" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="O9" s="8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -3872,7 +4051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -3909,8 +4088,18 @@
       <c r="L11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>75</v>
+      </c>
+      <c r="O11" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -3947,8 +4136,24 @@
       <c r="L12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N12" s="9"/>
+      <c r="O12" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -3985,8 +4190,29 @@
       <c r="L13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N13" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" s="7">
+        <v>3</v>
+      </c>
+      <c r="P13" s="7">
+        <v>945.75611583015075</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>315.25203861005025</v>
+      </c>
+      <c r="R13" s="7">
+        <v>48.960034456091059</v>
+      </c>
+      <c r="S13" s="7">
+        <v>2.9078715492971068E-11</v>
+      </c>
+      <c r="T13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -4023,8 +4249,22 @@
       <c r="L14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N14" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="O14" s="7">
+        <v>28</v>
+      </c>
+      <c r="P14" s="7">
+        <v>180.29107166984934</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>6.4389668453517626</v>
+      </c>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+    </row>
+    <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -4061,8 +4301,20 @@
       <c r="L15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N15" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="O15" s="8">
+        <v>31</v>
+      </c>
+      <c r="P15" s="8">
+        <v>1126.0471875000001</v>
+      </c>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+    </row>
+    <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -4100,7 +4352,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -4137,8 +4389,33 @@
       <c r="L17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N17" s="9"/>
+      <c r="O17" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q17" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="R17" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="S17" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="T17" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="U17" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="V17" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -4175,8 +4452,35 @@
       <c r="L18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="O18" s="11">
+        <v>34.002875122914062</v>
+      </c>
+      <c r="P18" s="7">
+        <v>2.6426593369900306</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>12.866915779482603</v>
+      </c>
+      <c r="R18" s="16">
+        <v>2.8240301965831147E-13</v>
+      </c>
+      <c r="S18" s="7">
+        <v>28.589632863691797</v>
+      </c>
+      <c r="T18" s="7">
+        <v>39.416117382136328</v>
+      </c>
+      <c r="U18" s="7">
+        <v>28.589632863691797</v>
+      </c>
+      <c r="V18" s="7">
+        <v>39.416117382136328</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -4213,8 +4517,35 @@
       <c r="L19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N19" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="O19" s="11">
+        <v>-3.7478725953382114E-2</v>
+      </c>
+      <c r="P19" s="7">
+        <v>9.6054221574033462E-3</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>-3.90183016833836</v>
+      </c>
+      <c r="R19" s="16">
+        <v>5.4640226580877677E-4</v>
+      </c>
+      <c r="S19" s="7">
+        <v>-5.7154541300565409E-2</v>
+      </c>
+      <c r="T19" s="7">
+        <v>-1.7802910606198815E-2</v>
+      </c>
+      <c r="U19" s="7">
+        <v>-5.7154541300565409E-2</v>
+      </c>
+      <c r="V19" s="7">
+        <v>-1.7802910606198815E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -4251,8 +4582,35 @@
       <c r="L20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N20" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="O20" s="11">
+        <v>-2.8785754138071864</v>
+      </c>
+      <c r="P20" s="7">
+        <v>0.90497053803057714</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>-3.1808498650924313</v>
+      </c>
+      <c r="R20" s="16">
+        <v>3.5740310794737246E-3</v>
+      </c>
+      <c r="S20" s="7">
+        <v>-4.7323235270233059</v>
+      </c>
+      <c r="T20" s="7">
+        <v>-1.0248273005910673</v>
+      </c>
+      <c r="U20" s="7">
+        <v>-4.7323235270233059</v>
+      </c>
+      <c r="V20" s="7">
+        <v>-1.0248273005910673</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -4289,8 +4647,35 @@
       <c r="L21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N21" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="O21" s="14">
+        <v>2.0837101303232957</v>
+      </c>
+      <c r="P21" s="8">
+        <v>1.3764201523049431</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>1.5138619750909124</v>
+      </c>
+      <c r="R21" s="17">
+        <v>0.14126823673653088</v>
+      </c>
+      <c r="S21" s="8">
+        <v>-0.73575873976904793</v>
+      </c>
+      <c r="T21" s="8">
+        <v>4.9031790004156388</v>
+      </c>
+      <c r="U21" s="8">
+        <v>-0.73575873976904793</v>
+      </c>
+      <c r="V21" s="8">
+        <v>4.9031790004156388</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -4328,7 +4713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -4366,7 +4751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -4404,7 +4789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -4442,7 +4827,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -4480,7 +4865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -4518,7 +4903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -4556,7 +4941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -4594,7 +4979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -4632,7 +5017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -4670,7 +5055,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -4747,7 +5132,11 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="O11:S11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>